<commit_message>
All tables 6 inputs
</commit_message>
<xml_diff>
--- a/sample_tables.xlsx
+++ b/sample_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danig\Documents\GitHub\Research\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FD0678-0D92-4713-AED7-80EBE1E77519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B262784-7E09-4787-8C8D-01B89C66DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{94E6D992-0F2D-4B9D-BD81-1E9E3BDAA891}"/>
+    <workbookView xWindow="-1150" yWindow="10690" windowWidth="22620" windowHeight="13500" activeTab="2" xr2:uid="{94E6D992-0F2D-4B9D-BD81-1E9E3BDAA891}"/>
   </bookViews>
   <sheets>
     <sheet name="VALUES" sheetId="10" r:id="rId1"/>
@@ -276,9 +276,6 @@
     <t>DS0_anime_color1.png</t>
   </si>
   <si>
-    <t xml:space="preserve">In the 'Watching' column, count how many values exceed the value of '80' </t>
-  </si>
-  <si>
     <t>DS0_anime_zebra2.png</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
   </si>
   <si>
     <t>DS0_anime_bar4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the 'On-Hold' column, count how many values exceed the value of '60' </t>
   </si>
   <si>
     <t xml:space="preserve">Determine which of the last 5 columns is most positively correlated with the column named 'Episodes' </t>
@@ -372,6 +366,12 @@
   <si>
     <t xml:space="preserve">In the 'Plan
  to Watch' column, find the anime with a value equal to '32' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 'Completed' column, count how many values exceed the value of '60' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 'On-Hold' column, count how many values exceed the value of '50' </t>
   </si>
 </sst>
 </file>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE75E392-E594-4944-8192-EC287EDF0175}">
   <dimension ref="A1:BP21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="118" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="I1" zoomScale="118" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,22 +1121,22 @@
         <v>1</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I2" s="13">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="J2" s="13">
         <v>0</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="L2" s="13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>15</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="3" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="13">
         <v>2</v>
@@ -1215,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L3" s="13">
         <v>6</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="4" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="13">
         <v>3</v>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L4" s="13">
         <v>5</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="5" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="13">
         <v>4</v>
@@ -1373,16 +1373,16 @@
         <v>22</v>
       </c>
       <c r="I5" s="13">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="J5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="L5" s="13">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="M5" s="13" t="s">
         <v>23</v>
@@ -1457,7 +1457,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
       <c r="K6" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L6" s="35" t="s">
         <v>35</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="7" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="35">
         <v>2</v>
@@ -1494,7 +1494,7 @@
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
       <c r="K7" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L7" s="35" t="s">
         <v>35</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="8" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="35">
         <v>3</v>
@@ -1531,7 +1531,7 @@
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
       <c r="K8" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L8" s="35" t="s">
         <v>35</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="9" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="35">
         <v>4</v>
@@ -1568,7 +1568,7 @@
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>35</v>
@@ -1603,22 +1603,22 @@
         <v>18</v>
       </c>
       <c r="I10" s="39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J10" s="39"/>
       <c r="K10" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="39" t="s">
         <v>79</v>
-      </c>
-      <c r="L10" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="M10" s="39" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="39">
         <v>2</v>
@@ -1642,22 +1642,22 @@
         <v>17</v>
       </c>
       <c r="I11" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J11" s="39"/>
       <c r="K11" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="M11" s="39" t="s">
         <v>83</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="M11" s="39" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="39">
         <v>3</v>
@@ -1681,22 +1681,22 @@
         <v>15</v>
       </c>
       <c r="I12" s="39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J12" s="39"/>
       <c r="K12" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="39" t="s">
         <v>87</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="M12" s="39" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="39">
         <v>4</v>
@@ -1720,17 +1720,17 @@
         <v>23</v>
       </c>
       <c r="I13" s="39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J13" s="39"/>
       <c r="K13" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="M13" s="39" t="s">
         <v>91</v>
-      </c>
-      <c r="L13" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="M13" s="39" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:68" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -1761,7 +1761,7 @@
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
       <c r="K14" s="45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L14" s="43">
         <v>28.896551724137932</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="15" spans="1:68" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="43">
         <v>2</v>
@@ -1798,10 +1798,10 @@
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
       <c r="K15" s="45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L15" s="43">
-        <v>52.310344827586206</v>
+        <v>52.310344827586199</v>
       </c>
       <c r="M15" s="43" t="s">
         <v>21</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="16" spans="1:68" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="43">
         <v>3</v>
@@ -1835,7 +1835,7 @@
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
       <c r="K16" s="45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L16" s="43">
         <v>63.068965517241381</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="17" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="43">
         <v>4</v>
@@ -1872,7 +1872,7 @@
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
       <c r="K17" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L17" s="43">
         <v>50.241379310344826</v>
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>59</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="13">
         <v>2</v>
@@ -1954,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L19" s="13" t="s">
         <v>51</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="13">
         <v>3</v>
@@ -1995,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L20" s="13" t="s">
         <v>41</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="13">
         <v>4</v>
@@ -2036,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L21" s="13" t="s">
         <v>57</v>
@@ -2054,7 +2054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700DFA64-0F6F-4CD7-8125-1F1598C774F9}">
   <dimension ref="A1:BP21"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="131" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="118" zoomScaleNormal="131" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -2454,19 +2454,19 @@
         <v>22</v>
       </c>
       <c r="I5" s="13">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5" s="15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">In the 'On-Hold' column, count how many values exceed the value of '50' </v>
+        <v xml:space="preserve">In the 'On-Hold' column, count how many values exceed the value of '53' </v>
       </c>
       <c r="L5" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M5" s="13" t="s">
         <v>23</v>
@@ -3366,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DCBDE1-CBA9-443B-9602-67C1589E4840}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:N1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="61" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4780,7 +4780,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:N33"/>
+      <selection sqref="A1:N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6220,8 +6220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D67901-18CB-4D03-BA2F-791ED69C5872}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7630,7 +7630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEBFF06-1EA3-423A-B086-D35C0BA46852}">
   <dimension ref="B1:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:N32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9142,6 +9144,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J31">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DCE78AD6-162E-45F4-86E6-A93F2872876F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -9154,18 +9168,6 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="8">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{DCE78AD6-162E-45F4-86E6-A93F2872876F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
     <cfRule type="colorScale" priority="37">
@@ -9234,6 +9236,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L31">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5CC836EA-CF00-4BFA-AB79-D15CE7AFB123}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -9246,7 +9260,29 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="4">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L32">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M31">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9254,32 +9290,10 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5CC836EA-CF00-4BFA-AB79-D15CE7AFB123}</x14:id>
+          <x14:id>{CF1529C8-7D17-45AC-B706-28DFDA309DCC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L32">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M31">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -9289,18 +9303,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{D866D858-121D-4437-881F-161079AF9745}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CF1529C8-7D17-45AC-B706-28DFDA309DCC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -9481,20 +9483,20 @@
           <xm:sqref>I3:I31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5A10EA8C-F875-4772-898D-BCC0A6FAC3A8}">
+          <x14:cfRule type="dataBar" id="{DCE78AD6-162E-45F4-86E6-A93F2872876F}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="min"/>
-              <x14:cfvo type="max"/>
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
               <x14:borderColor rgb="FFFF555A"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:negativeBorderColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{DCE78AD6-162E-45F4-86E6-A93F2872876F}">
+          <x14:cfRule type="dataBar" id="{5A10EA8C-F875-4772-898D-BCC0A6FAC3A8}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
+              <x14:cfvo type="min"/>
+              <x14:cfvo type="max"/>
               <x14:borderColor rgb="FFFF555A"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:negativeBorderColor rgb="FFFF0000"/>
@@ -9527,6 +9529,16 @@
           <xm:sqref>K3:K31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5CC836EA-CF00-4BFA-AB79-D15CE7AFB123}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
           <x14:cfRule type="dataBar" id="{0B9AB73A-9BBF-4508-BF39-FFB3A0251037}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="min"/>
@@ -9537,7 +9549,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{5CC836EA-CF00-4BFA-AB79-D15CE7AFB123}">
+          <xm:sqref>L3:L31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CF1529C8-7D17-45AC-B706-28DFDA309DCC}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -9547,23 +9562,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L3:L31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D866D858-121D-4437-881F-161079AF9745}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="min"/>
               <x14:cfvo type="max"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{CF1529C8-7D17-45AC-B706-28DFDA309DCC}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
               <x14:borderColor rgb="FFFF555A"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:negativeBorderColor rgb="FFFF0000"/>

</xml_diff>